<commit_message>
API ?꾩껜 JSON 諛섑솚, 30??DOM ?꾩쟻 ?쒓굅, start-server.ps1 踰꾩쟾 ?쒖떆, 湲고? ?뺣━
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/.source/Card/국민카드_김찬식_2021-2025.xlsx
+++ b/.source/Card/국민카드_김찬식_2021-2025.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d251688e3d9c1650/Cursor_AI_Project/MYBCINFO/MYBCCARD/Source/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d251688e3d9c1650/Cursor/MyInfo/.source/Card/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{516B17B3-5C6A-4443-8AD5-A15C0ADC2680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26ECCA7E-2144-4555-8927-FAD85D6AFB21}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{516B17B3-5C6A-4443-8AD5-A15C0ADC2680}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB3C6E6E-325E-434B-B021-78E49C7B9D24}"/>
   <bookViews>
-    <workbookView xWindow="38730" yWindow="2055" windowWidth="28320" windowHeight="12720" xr2:uid="{02FE0329-166C-41D0-A357-80C5F33B6BA2}"/>
+    <workbookView xWindow="6900" yWindow="8160" windowWidth="28320" windowHeight="12720" xr2:uid="{02FE0329-166C-41D0-A357-80C5F33B6BA2}"/>
   </bookViews>
   <sheets>
     <sheet name="과거이용내역" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">과거이용내역!$I$1:$I$157</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">과거이용내역!$A$1:$M$157</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
@@ -2204,10 +2205,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51198B0E-F92B-466D-BCD9-0F69F5D6D0A3}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:M157"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="75" zoomScaleNormal="80" zoomScaleSheetLayoutView="75" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2265,7 +2267,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -2306,7 +2308,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -2347,7 +2349,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -2388,7 +2390,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -2429,7 +2431,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>31</v>
       </c>
@@ -2470,7 +2472,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -2511,7 +2513,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>39</v>
       </c>
@@ -2552,7 +2554,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>44</v>
       </c>
@@ -2593,7 +2595,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -2634,7 +2636,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>54</v>
       </c>
@@ -2675,7 +2677,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>59</v>
       </c>
@@ -2716,7 +2718,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>64</v>
       </c>
@@ -2757,7 +2759,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -2798,7 +2800,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>74</v>
       </c>
@@ -2839,7 +2841,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>79</v>
       </c>
@@ -2880,7 +2882,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>84</v>
       </c>
@@ -2921,7 +2923,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>87</v>
       </c>
@@ -2962,7 +2964,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>90</v>
       </c>
@@ -3003,7 +3005,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>93</v>
       </c>
@@ -3044,7 +3046,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>98</v>
       </c>
@@ -3085,7 +3087,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>103</v>
       </c>
@@ -3126,7 +3128,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>108</v>
       </c>
@@ -3167,7 +3169,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>113</v>
       </c>
@@ -3208,7 +3210,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>118</v>
       </c>
@@ -3249,7 +3251,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>121</v>
       </c>
@@ -3290,7 +3292,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>126</v>
       </c>
@@ -3331,7 +3333,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>131</v>
       </c>
@@ -3372,7 +3374,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>136</v>
       </c>
@@ -3454,7 +3456,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>142</v>
       </c>
@@ -3495,7 +3497,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>146</v>
       </c>
@@ -3536,7 +3538,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>151</v>
       </c>
@@ -3577,7 +3579,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>156</v>
       </c>
@@ -3618,7 +3620,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>161</v>
       </c>
@@ -3659,7 +3661,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>164</v>
       </c>
@@ -3700,7 +3702,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>167</v>
       </c>
@@ -3823,7 +3825,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>178</v>
       </c>
@@ -3864,7 +3866,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>183</v>
       </c>
@@ -3905,7 +3907,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>188</v>
       </c>
@@ -3946,7 +3948,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>193</v>
       </c>
@@ -4028,7 +4030,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>203</v>
       </c>
@@ -4069,7 +4071,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>206</v>
       </c>
@@ -4110,7 +4112,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>209</v>
       </c>
@@ -4151,7 +4153,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>212</v>
       </c>
@@ -4192,7 +4194,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>216</v>
       </c>
@@ -4233,7 +4235,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>219</v>
       </c>
@@ -4274,7 +4276,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>224</v>
       </c>
@@ -4315,7 +4317,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>227</v>
       </c>
@@ -4397,7 +4399,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>234</v>
       </c>
@@ -4438,7 +4440,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>237</v>
       </c>
@@ -4479,7 +4481,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>240</v>
       </c>
@@ -4520,7 +4522,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>243</v>
       </c>
@@ -4561,7 +4563,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>246</v>
       </c>
@@ -4602,7 +4604,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>251</v>
       </c>
@@ -4643,7 +4645,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>254</v>
       </c>
@@ -4684,7 +4686,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>259</v>
       </c>
@@ -4725,7 +4727,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>264</v>
       </c>
@@ -4766,7 +4768,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>269</v>
       </c>
@@ -4807,7 +4809,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>274</v>
       </c>
@@ -4848,7 +4850,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>279</v>
       </c>
@@ -4889,7 +4891,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>282</v>
       </c>
@@ -4930,7 +4932,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="67" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>287</v>
       </c>
@@ -4971,7 +4973,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="68" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>292</v>
       </c>
@@ -5012,7 +5014,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="69" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>295</v>
       </c>
@@ -5053,7 +5055,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="70" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>298</v>
       </c>
@@ -5094,7 +5096,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="71" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>301</v>
       </c>
@@ -5135,7 +5137,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="72" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>306</v>
       </c>
@@ -5176,7 +5178,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="73" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>309</v>
       </c>
@@ -5217,7 +5219,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="74" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>312</v>
       </c>
@@ -5258,7 +5260,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="75" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>317</v>
       </c>
@@ -5299,7 +5301,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="76" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>320</v>
       </c>
@@ -5381,7 +5383,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="78" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>325</v>
       </c>
@@ -5422,7 +5424,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="79" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>328</v>
       </c>
@@ -5463,7 +5465,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="80" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>331</v>
       </c>
@@ -5504,7 +5506,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="81" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>336</v>
       </c>
@@ -5545,7 +5547,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="82" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>339</v>
       </c>
@@ -5586,7 +5588,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="83" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>344</v>
       </c>
@@ -5627,7 +5629,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="84" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>347</v>
       </c>
@@ -5668,7 +5670,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="85" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>350</v>
       </c>
@@ -5709,7 +5711,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="86" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>353</v>
       </c>
@@ -5750,7 +5752,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="87" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>356</v>
       </c>
@@ -5791,7 +5793,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="88" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>359</v>
       </c>
@@ -5832,7 +5834,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="89" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>362</v>
       </c>
@@ -5873,7 +5875,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="90" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>365</v>
       </c>
@@ -5914,7 +5916,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="91" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>368</v>
       </c>
@@ -5955,7 +5957,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="92" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>371</v>
       </c>
@@ -5996,7 +5998,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="93" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>374</v>
       </c>
@@ -6037,7 +6039,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="94" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>379</v>
       </c>
@@ -6078,7 +6080,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="95" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>384</v>
       </c>
@@ -6119,7 +6121,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="96" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>387</v>
       </c>
@@ -6160,7 +6162,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="97" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>392</v>
       </c>
@@ -6242,7 +6244,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="99" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>397</v>
       </c>
@@ -6283,7 +6285,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="100" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>402</v>
       </c>
@@ -6324,7 +6326,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="101" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>404</v>
       </c>
@@ -6365,7 +6367,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="102" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>407</v>
       </c>
@@ -6406,7 +6408,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="103" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>410</v>
       </c>
@@ -6447,7 +6449,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="104" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>413</v>
       </c>
@@ -6488,7 +6490,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="105" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>416</v>
       </c>
@@ -6529,7 +6531,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="106" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>419</v>
       </c>
@@ -6570,7 +6572,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="107" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>422</v>
       </c>
@@ -6611,7 +6613,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="108" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>427</v>
       </c>
@@ -6652,7 +6654,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="109" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>430</v>
       </c>
@@ -6693,7 +6695,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="110" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>433</v>
       </c>
@@ -6734,7 +6736,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="111" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>437</v>
       </c>
@@ -6775,7 +6777,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="112" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>441</v>
       </c>
@@ -6816,7 +6818,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="113" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>444</v>
       </c>
@@ -6857,7 +6859,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="114" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>447</v>
       </c>
@@ -6898,7 +6900,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="115" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>450</v>
       </c>
@@ -6939,7 +6941,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="116" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>453</v>
       </c>
@@ -6980,7 +6982,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="117" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>456</v>
       </c>
@@ -7021,7 +7023,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="118" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>461</v>
       </c>
@@ -7062,7 +7064,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="119" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>464</v>
       </c>
@@ -7103,7 +7105,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="120" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>467</v>
       </c>
@@ -7185,7 +7187,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="122" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>472</v>
       </c>
@@ -7226,7 +7228,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="123" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>475</v>
       </c>
@@ -7267,7 +7269,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="124" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>478</v>
       </c>
@@ -7308,7 +7310,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="125" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>483</v>
       </c>
@@ -7349,7 +7351,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="126" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>486</v>
       </c>
@@ -7390,7 +7392,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="127" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>489</v>
       </c>
@@ -7431,7 +7433,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="128" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>492</v>
       </c>
@@ -7472,7 +7474,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="129" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>495</v>
       </c>
@@ -7513,7 +7515,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="130" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>498</v>
       </c>
@@ -7595,7 +7597,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="132" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>503</v>
       </c>
@@ -7636,7 +7638,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="133" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>506</v>
       </c>
@@ -7677,7 +7679,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="134" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>509</v>
       </c>
@@ -7759,7 +7761,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="136" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>514</v>
       </c>
@@ -7800,7 +7802,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="137" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>517</v>
       </c>
@@ -7841,7 +7843,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="138" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>520</v>
       </c>
@@ -7882,7 +7884,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="139" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>523</v>
       </c>
@@ -7923,7 +7925,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="140" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>527</v>
       </c>
@@ -7964,7 +7966,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="141" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>532</v>
       </c>
@@ -8005,7 +8007,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="142" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>537</v>
       </c>
@@ -8046,7 +8048,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="143" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>542</v>
       </c>
@@ -8087,7 +8089,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="144" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>547</v>
       </c>
@@ -8128,7 +8130,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="145" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>552</v>
       </c>
@@ -8169,7 +8171,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="146" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>555</v>
       </c>
@@ -8210,7 +8212,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="147" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>558</v>
       </c>
@@ -8251,7 +8253,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="148" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>563</v>
       </c>
@@ -8292,7 +8294,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="149" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>566</v>
       </c>
@@ -8333,7 +8335,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="150" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>569</v>
       </c>
@@ -8374,7 +8376,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="151" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>572</v>
       </c>
@@ -8415,7 +8417,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="152" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>575</v>
       </c>
@@ -8456,7 +8458,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="153" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>578</v>
       </c>
@@ -8497,7 +8499,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="154" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>581</v>
       </c>
@@ -8538,7 +8540,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="155" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>584</v>
       </c>
@@ -8579,7 +8581,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="156" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>587</v>
       </c>
@@ -8620,7 +8622,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="157" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:13" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>591</v>
       </c>
@@ -8662,6 +8664,15 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="I1:I157" xr:uid="{51198B0E-F92B-466D-BCD9-0F69F5D6D0A3}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="300"/>
+        <filter val="500"/>
+        <filter val="630"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.39370078740157483"/>
   <pageSetup paperSize="9" scale="53" orientation="portrait" r:id="rId1"/>

</xml_diff>